<commit_message>
almost done with fec ecosite tool
</commit_message>
<xml_diff>
--- a/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
+++ b/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p2t_ArcMap10_Tools\Misc\FEC_EcositePredictor\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF143C2-6192-407D-BE21-7F115F22CD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99D7A4A-1AC3-458F-ACBB-43029740D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81CC09A0-CCBA-490A-882D-74783881A46D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81CC09A0-CCBA-490A-882D-74783881A46D}"/>
   </bookViews>
   <sheets>
     <sheet name="Central Ontario FEC" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C85DBCD6-18B6-4261-A6AC-DBD344816A20}</author>
+    <author>tc={030EB0EE-1CB5-4423-8EAF-3ED500C1FC44}</author>
+    <author>tc={55A9BCD1-1BE8-4055-B4CE-3AF7EAE06849}</author>
+  </authors>
+  <commentList>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{C85DBCD6-18B6-4261-A6AC-DBD344816A20}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    QR+OW+OB</t>
+      </text>
+    </comment>
+    <comment ref="AG3" authorId="1" shapeId="0" xr:uid="{030EB0EE-1CB5-4423-8EAF-3ED500C1FC44}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    SC but turn the values to 1, 2 or 3</t>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="2" shapeId="0" xr:uid="{55A9BCD1-1BE8-4055-B4CE-3AF7EAE06849}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    J4 is AW+CH not AB+EW</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="156">
   <si>
@@ -148,9 +184,6 @@
     <t>BE</t>
   </si>
   <si>
-    <t>OR</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
@@ -508,13 +541,16 @@
   </si>
   <si>
     <t>FEC NAME</t>
+  </si>
+  <si>
+    <t>Oak</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +597,12 @@
       <color theme="1"/>
       <name val="Daytona"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2596,6 +2638,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Kim, Daniel (MNR)" id="{58E23E94-745B-476D-AAC4-4B4D22141E06}" userId="S::Daniel.Kim2@ontario.ca::6a941af3-110c-4c3c-b425-309817122f3e" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2891,15 +2939,29 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G3" dT="2024-12-16T14:07:46.63" personId="{58E23E94-745B-476D-AAC4-4B4D22141E06}" id="{C85DBCD6-18B6-4261-A6AC-DBD344816A20}">
+    <text>QR+OW+OB</text>
+  </threadedComment>
+  <threadedComment ref="AG3" dT="2024-12-16T13:57:00.04" personId="{58E23E94-745B-476D-AAC4-4B4D22141E06}" id="{030EB0EE-1CB5-4423-8EAF-3ED500C1FC44}">
+    <text>SC but turn the values to 1, 2 or 3</text>
+  </threadedComment>
+  <threadedComment ref="N5" dT="2024-12-16T13:59:57.37" personId="{58E23E94-745B-476D-AAC4-4B4D22141E06}" id="{55A9BCD1-1BE8-4055-B4CE-3AF7EAE06849}">
+    <text>J4 is AW+CH not AB+EW</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B514C5FF-EF35-48A4-A3CD-10618138AC7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B514C5FF-EF35-48A4-A3CD-10618138AC7D}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B2:CP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN25" sqref="AN25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,90 +3090,90 @@
         <v>35</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -3203,7 +3265,7 @@
     </row>
     <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="8">
         <f>C4</f>
@@ -5887,106 +5949,106 @@
         <v>0</v>
       </c>
       <c r="C34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="P34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="R34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="S34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="V34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="W34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="X34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH34" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="N34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="O34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="P34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="R34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="T34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="U34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="V34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="W34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="X34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH34" s="14" t="s">
+      <c r="AJ34" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="AJ34" s="15" t="s">
+      <c r="AK34" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="AK34" s="15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.25">
@@ -6122,10 +6184,10 @@
         <v>65.1911165480481</v>
       </c>
       <c r="AJ35" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK35" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="AK35" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.25">
@@ -6261,10 +6323,10 @@
         <v>-318.97210623138238</v>
       </c>
       <c r="AJ36" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK36" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="AK36" s="19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.25">
@@ -6400,10 +6462,10 @@
         <v>53.78180921763736</v>
       </c>
       <c r="AJ37" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK37" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="AK37" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.25">
@@ -6539,10 +6601,10 @@
         <v>65.954230106248232</v>
       </c>
       <c r="AJ38" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK38" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="AK38" s="19" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.25">
@@ -6678,10 +6740,10 @@
         <v>46.988224844585673</v>
       </c>
       <c r="AJ39" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK39" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="AK39" s="19" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.25">
@@ -6817,10 +6879,10 @@
         <v>56.208465760547128</v>
       </c>
       <c r="AJ40" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK40" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="AK40" s="19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="41" spans="2:37" x14ac:dyDescent="0.25">
@@ -6956,10 +7018,10 @@
         <v>58.927795657300578</v>
       </c>
       <c r="AJ41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK41" s="19" t="s">
         <v>81</v>
-      </c>
-      <c r="AK41" s="19" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="42" spans="2:37" x14ac:dyDescent="0.25">
@@ -7095,10 +7157,10 @@
         <v>60.800163610039078</v>
       </c>
       <c r="AJ42" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK42" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="AK42" s="19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="43" spans="2:37" x14ac:dyDescent="0.25">
@@ -7234,10 +7296,10 @@
         <v>72.411227375899557</v>
       </c>
       <c r="AJ43" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK43" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="AK43" s="19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="44" spans="2:37" x14ac:dyDescent="0.25">
@@ -7373,10 +7435,10 @@
         <v>65.454584271852539</v>
       </c>
       <c r="AJ44" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK44" s="19" t="s">
         <v>87</v>
-      </c>
-      <c r="AK44" s="19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="45" spans="2:37" x14ac:dyDescent="0.25">
@@ -7512,10 +7574,10 @@
         <v>67.313652475759142</v>
       </c>
       <c r="AJ45" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK45" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="AK45" s="19" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="46" spans="2:37" x14ac:dyDescent="0.25">
@@ -7651,10 +7713,10 @@
         <v>65.837910867986608</v>
       </c>
       <c r="AJ46" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK46" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="AK46" s="19" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:37" x14ac:dyDescent="0.25">
@@ -7790,10 +7852,10 @@
         <v>61.22410213483721</v>
       </c>
       <c r="AJ47" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK47" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="AK47" s="19" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="48" spans="2:37" x14ac:dyDescent="0.25">
@@ -7929,10 +7991,10 @@
         <v>45.2151622744734</v>
       </c>
       <c r="AJ48" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK48" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="AK48" s="19" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="49" spans="2:94" x14ac:dyDescent="0.25">
@@ -8068,10 +8130,10 @@
         <v>62.989231628623415</v>
       </c>
       <c r="AJ49" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK49" s="19" t="s">
         <v>97</v>
-      </c>
-      <c r="AK49" s="19" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="50" spans="2:94" x14ac:dyDescent="0.25">
@@ -8207,10 +8269,10 @@
         <v>16.065230548732501</v>
       </c>
       <c r="AJ50" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK50" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="AK50" s="19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="51" spans="2:94" x14ac:dyDescent="0.25">
@@ -8346,10 +8408,10 @@
         <v>71.652186026259983</v>
       </c>
       <c r="AJ51" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK51" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="AK51" s="19" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="52" spans="2:94" x14ac:dyDescent="0.25">
@@ -8485,10 +8547,10 @@
         <v>92.460907307605481</v>
       </c>
       <c r="AJ52" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK52" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="AK52" s="19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53" spans="2:94" x14ac:dyDescent="0.25">
@@ -8624,10 +8686,10 @@
         <v>42.476107681155128</v>
       </c>
       <c r="AJ53" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK53" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="AK53" s="19" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="54" spans="2:94" x14ac:dyDescent="0.25">
@@ -8763,10 +8825,10 @@
         <v>110.84018840898702</v>
       </c>
       <c r="AJ54" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK54" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="AK54" s="19" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="55" spans="2:94" x14ac:dyDescent="0.25">
@@ -8902,10 +8964,10 @@
         <v>-17.656448559923739</v>
       </c>
       <c r="AJ55" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK55" s="19" t="s">
         <v>109</v>
-      </c>
-      <c r="AK55" s="19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="56" spans="2:94" x14ac:dyDescent="0.25">
@@ -9041,10 +9103,10 @@
         <v>4.8082557829230552</v>
       </c>
       <c r="AJ56" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK56" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="AK56" s="19" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="57" spans="2:94" x14ac:dyDescent="0.25">
@@ -9180,10 +9242,10 @@
         <v>56.646690123903454</v>
       </c>
       <c r="AJ57" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK57" s="19" t="s">
         <v>113</v>
-      </c>
-      <c r="AK57" s="19" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:94" x14ac:dyDescent="0.25">
@@ -9319,10 +9381,10 @@
         <v>55.93473091283559</v>
       </c>
       <c r="AJ58" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK58" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="AK58" s="19" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="59" spans="2:94" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9458,129 +9520,129 @@
         <v>53.169545146753933</v>
       </c>
       <c r="AJ59" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK59" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="AK59" s="19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="60" spans="2:94" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BJ60" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="BK60" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="BK60" s="23" t="s">
+      <c r="BL60" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="BL60" s="23" t="s">
+      <c r="BM60" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="BM60" s="23" t="s">
+      <c r="BN60" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="BN60" s="23" t="s">
+      <c r="BO60" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="BO60" s="23" t="s">
+      <c r="BP60" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="BP60" s="23" t="s">
+      <c r="BQ60" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="BQ60" s="23" t="s">
+      <c r="BR60" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="BR60" s="23" t="s">
+      <c r="BS60" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="BS60" s="23" t="s">
+      <c r="BT60" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="BT60" s="23" t="s">
+      <c r="BU60" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="BU60" s="23" t="s">
+      <c r="BV60" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="BV60" s="23" t="s">
+      <c r="BW60" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="BW60" s="23" t="s">
+      <c r="BX60" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="BX60" s="23" t="s">
+      <c r="BY60" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="BY60" s="23" t="s">
+      <c r="BZ60" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="BZ60" s="23" t="s">
+      <c r="CA60" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="CA60" s="23" t="s">
+      <c r="CB60" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="CB60" s="23" t="s">
+      <c r="CC60" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="CC60" s="23" t="s">
+      <c r="CD60" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="CD60" s="23" t="s">
+      <c r="CE60" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="CE60" s="23" t="s">
+      <c r="CF60" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="CF60" s="23" t="s">
+      <c r="CG60" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="CG60" s="23" t="s">
+      <c r="CH60" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="CH60" s="23" t="s">
+      <c r="CI60" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="CI60" s="23" t="s">
+      <c r="CJ60" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="CJ60" s="23" t="s">
+      <c r="CK60" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="CK60" s="23" t="s">
+      <c r="CL60" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="CL60" s="23" t="s">
+      <c r="CM60" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="CM60" s="23" t="s">
+      <c r="CN60" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="CN60" s="23" t="s">
+      <c r="CO60" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="CO60" s="23" t="s">
+      <c r="CP60" s="23" t="s">
         <v>150</v>
-      </c>
-      <c r="CP60" s="23" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="61" spans="2:94" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B61" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C61" s="27"/>
       <c r="D61" s="28"/>
       <c r="E61" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H61" s="36"/>
       <c r="I61" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J61" s="36"/>
       <c r="BJ61" s="24">
@@ -12150,6 +12212,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -14731,10 +14794,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -14742,7 +14805,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -14750,7 +14813,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14758,7 +14821,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -14766,7 +14829,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -14774,7 +14837,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -14782,7 +14845,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -14790,7 +14853,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -14798,7 +14861,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -14806,7 +14869,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -14814,7 +14877,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -14822,7 +14885,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -14830,7 +14893,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -14838,7 +14901,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -14846,7 +14909,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -14854,7 +14917,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -14862,7 +14925,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -14870,7 +14933,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -14878,7 +14941,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -14886,7 +14949,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -14894,7 +14957,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -14902,7 +14965,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -14910,7 +14973,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -14918,7 +14981,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -14926,7 +14989,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14934,7 +14997,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new fec_ecositePredictor excel file
</commit_message>
<xml_diff>
--- a/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
+++ b/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/glen_watt_ontario_ca/Documents/Laptop_Feb2024/OLD_GROWTH/Dawn_B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MNR_SR_External\GI_MGMT\GISupport\OldGrowthAnalysis\Documents_GWatt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="344" documentId="8_{A14C0133-3C12-4172-A6DC-864A58E6BE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D75E0097-21C7-46F8-9E7F-D193925BABD2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D49DB22-8E40-4DB3-B13C-5C8D86E14300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{81CC09A0-CCBA-490A-882D-74783881A46D}"/>
   </bookViews>
@@ -3138,7 +3138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BAB770-D548-4A89-9CE4-B3603514F2DA}">
   <dimension ref="B1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3270,13 +3270,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I4" s="30">
         <v>0</v>
       </c>
       <c r="J4" s="30">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="K4" s="30">
         <v>0</v>
@@ -3321,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="Z4" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -3409,12 +3409,12 @@
     <row r="9" spans="2:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K9" s="44">
         <f>'Central Ontario FEC'!G62</f>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L9" s="45"/>
       <c r="M9" s="46" t="str">
         <f>'Central Ontario FEC'!I62</f>
-        <v>CeSbL</v>
+        <v>PoBw</v>
       </c>
       <c r="N9" s="45"/>
     </row>
@@ -3439,9 +3439,7 @@
   </sheetPr>
   <dimension ref="B2:CP85"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3727,7 +3725,7 @@
       </c>
       <c r="U4" s="6">
         <f>'User Entry'!H4</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V4" s="6">
         <f>'User Entry'!I4</f>
@@ -3735,14 +3733,14 @@
       </c>
       <c r="W4" s="6">
         <f>'User Entry'!J4</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="X4" s="6">
         <f>D4+E4+F4</f>
         <v>0</v>
       </c>
       <c r="Y4" s="6">
-        <f>G4+H4+I4+J4+K4+N4</f>
+        <f>G4+H4+I4+J4+K4+N4+'User Entry'!X4</f>
         <v>0</v>
       </c>
       <c r="Z4" s="6">
@@ -3751,7 +3749,7 @@
       </c>
       <c r="AA4" s="6">
         <f>O4+P4+Q4+R4+S4+T4+U4+V4+W4</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
@@ -3760,11 +3758,11 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6">
         <f>'User Entry'!Z4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AP4" s="25">
         <f>SUM(D4:M4,O4:V4)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:42" x14ac:dyDescent="0.25">
@@ -3816,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="8">
-        <f>IF(AND(O4&lt;30,P4&lt;20,G4&lt;20, K4&lt;20),N4^0.5,0)</f>
+        <f>IF(AND(O4&lt;30,P4&lt;20,Q4&lt;20,G4&lt;20, F4&lt;20,K4&lt;20),N4^0.5,0)</f>
         <v>0</v>
       </c>
       <c r="O5" s="8">
@@ -3845,7 +3843,7 @@
       </c>
       <c r="U5" s="8">
         <f t="shared" si="0"/>
-        <v>3.1622776601683795</v>
+        <v>0</v>
       </c>
       <c r="V5" s="8">
         <f t="shared" si="0"/>
@@ -3853,7 +3851,7 @@
       </c>
       <c r="W5" s="8">
         <f>IF(OR(O4&gt;10,P4&gt;10,Q4&gt;10,G4&gt;10,K4&gt;10),0,W4^0.5)</f>
-        <v>9.4868329805051381</v>
+        <v>0</v>
       </c>
       <c r="X5" s="8">
         <f t="shared" si="0"/>
@@ -3869,7 +3867,7 @@
       </c>
       <c r="AA5" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="8">
         <f>IF(P4&gt;=50,1,0)</f>
@@ -3893,7 +3891,7 @@
       </c>
       <c r="AG5" s="8">
         <f>IF(AG4&lt;=1,1,IF(AG4=2,2,IF(AG4&gt;=3,3)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:42" x14ac:dyDescent="0.25">
@@ -6633,7 +6631,7 @@
       </c>
       <c r="U35" s="8">
         <f t="shared" si="1"/>
-        <v>-22.478355046221687</v>
+        <v>0</v>
       </c>
       <c r="V35" s="8">
         <f t="shared" si="1"/>
@@ -6641,7 +6639,7 @@
       </c>
       <c r="W35" s="8">
         <f t="shared" si="1"/>
-        <v>9.3363718094343273</v>
+        <v>0</v>
       </c>
       <c r="X35" s="8">
         <f t="shared" si="1"/>
@@ -6657,7 +6655,7 @@
       </c>
       <c r="AA35" s="8">
         <f t="shared" si="1"/>
-        <v>262.03910000000002</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="8">
         <f t="shared" si="1"/>
@@ -6681,11 +6679,11 @@
       </c>
       <c r="AG35" s="17">
         <f t="shared" si="1"/>
-        <v>61.134419999999999</v>
+        <v>30.567209999999999</v>
       </c>
       <c r="AH35" s="18">
         <f>SUM(C35:AG35)</f>
-        <v>110.98611676321266</v>
+        <v>-168.47821000000002</v>
       </c>
       <c r="AJ35" s="19" t="s">
         <v>69</v>
@@ -6772,7 +6770,7 @@
       </c>
       <c r="U36" s="8">
         <f t="shared" si="1"/>
-        <v>-29.764780362451862</v>
+        <v>0</v>
       </c>
       <c r="V36" s="8">
         <f t="shared" si="1"/>
@@ -6780,7 +6778,7 @@
       </c>
       <c r="W36" s="8">
         <f t="shared" si="1"/>
-        <v>5.0165424117613115</v>
+        <v>0</v>
       </c>
       <c r="X36" s="8">
         <f t="shared" si="1"/>
@@ -6796,7 +6794,7 @@
       </c>
       <c r="AA36" s="8">
         <f t="shared" si="1"/>
-        <v>309.8802</v>
+        <v>0</v>
       </c>
       <c r="AB36" s="8">
         <f t="shared" si="1"/>
@@ -6820,11 +6818,11 @@
       </c>
       <c r="AG36" s="17">
         <f t="shared" si="1"/>
-        <v>52.947279999999999</v>
+        <v>26.47364</v>
       </c>
       <c r="AH36" s="18">
         <f t="shared" ref="AH36:AH59" si="3">SUM(C36:AG36)</f>
-        <v>-262.62484795069059</v>
+        <v>-574.23044999999991</v>
       </c>
       <c r="AJ36" s="19" t="s">
         <v>71</v>
@@ -6911,7 +6909,7 @@
       </c>
       <c r="U37" s="8">
         <f t="shared" si="1"/>
-        <v>-22.275463311545288</v>
+        <v>0</v>
       </c>
       <c r="V37" s="8">
         <f t="shared" si="1"/>
@@ -6919,7 +6917,7 @@
       </c>
       <c r="W37" s="8">
         <f t="shared" si="1"/>
-        <v>18.868741588245889</v>
+        <v>0</v>
       </c>
       <c r="X37" s="8">
         <f t="shared" si="1"/>
@@ -6935,7 +6933,7 @@
       </c>
       <c r="AA37" s="8">
         <f t="shared" si="1"/>
-        <v>255.84479999999999</v>
+        <v>0</v>
       </c>
       <c r="AB37" s="8">
         <f t="shared" si="1"/>
@@ -6959,11 +6957,11 @@
       </c>
       <c r="AG37" s="17">
         <f t="shared" si="1"/>
-        <v>72.915019999999998</v>
+        <v>36.457509999999999</v>
       </c>
       <c r="AH37" s="18">
         <f t="shared" si="3"/>
-        <v>105.7277582767006</v>
+        <v>-183.16782999999998</v>
       </c>
       <c r="AJ37" s="19" t="s">
         <v>73</v>
@@ -7050,7 +7048,7 @@
       </c>
       <c r="U38" s="8">
         <f t="shared" si="1"/>
-        <v>-15.661021998100891</v>
+        <v>0</v>
       </c>
       <c r="V38" s="8">
         <f t="shared" si="1"/>
@@ -7058,7 +7056,7 @@
       </c>
       <c r="W38" s="8">
         <f t="shared" si="1"/>
-        <v>6.474004562556317</v>
+        <v>0</v>
       </c>
       <c r="X38" s="8">
         <f t="shared" si="1"/>
@@ -7074,7 +7072,7 @@
       </c>
       <c r="AA38" s="8">
         <f t="shared" si="1"/>
-        <v>267.85270000000003</v>
+        <v>0</v>
       </c>
       <c r="AB38" s="8">
         <f t="shared" si="1"/>
@@ -7098,11 +7096,11 @@
       </c>
       <c r="AG38" s="17">
         <f t="shared" si="1"/>
-        <v>60.411059999999999</v>
+        <v>30.20553</v>
       </c>
       <c r="AH38" s="18">
         <f t="shared" si="3"/>
-        <v>97.513692564455454</v>
+        <v>-191.35751999999999</v>
       </c>
       <c r="AJ38" s="19" t="s">
         <v>75</v>
@@ -7189,7 +7187,7 @@
       </c>
       <c r="U39" s="8">
         <f t="shared" si="1"/>
-        <v>-30.590988646724053</v>
+        <v>0</v>
       </c>
       <c r="V39" s="8">
         <f t="shared" si="1"/>
@@ -7197,7 +7195,7 @@
       </c>
       <c r="W39" s="8">
         <f t="shared" si="1"/>
-        <v>25.900856535045321</v>
+        <v>0</v>
       </c>
       <c r="X39" s="8">
         <f t="shared" si="1"/>
@@ -7213,7 +7211,7 @@
       </c>
       <c r="AA39" s="8">
         <f t="shared" si="1"/>
-        <v>283.1164</v>
+        <v>0</v>
       </c>
       <c r="AB39" s="8">
         <f t="shared" si="1"/>
@@ -7237,11 +7235,11 @@
       </c>
       <c r="AG39" s="17">
         <f t="shared" si="1"/>
-        <v>66.473579999999998</v>
+        <v>33.236789999999999</v>
       </c>
       <c r="AH39" s="18">
         <f t="shared" si="3"/>
-        <v>104.32822788832127</v>
+        <v>-207.33483000000001</v>
       </c>
       <c r="AJ39" s="19" t="s">
         <v>77</v>
@@ -7328,7 +7326,7 @@
       </c>
       <c r="U40" s="8">
         <f t="shared" si="1"/>
-        <v>-26.469971645545829</v>
+        <v>0</v>
       </c>
       <c r="V40" s="8">
         <f t="shared" si="1"/>
@@ -7336,7 +7334,7 @@
       </c>
       <c r="W40" s="8">
         <f t="shared" si="1"/>
-        <v>19.287016054356361</v>
+        <v>0</v>
       </c>
       <c r="X40" s="8">
         <f t="shared" si="1"/>
@@ -7352,7 +7350,7 @@
       </c>
       <c r="AA40" s="8">
         <f t="shared" si="1"/>
-        <v>278.85309999999998</v>
+        <v>0</v>
       </c>
       <c r="AB40" s="8">
         <f t="shared" si="1"/>
@@ -7376,11 +7374,11 @@
       </c>
       <c r="AG40" s="17">
         <f t="shared" si="1"/>
-        <v>58.141379999999998</v>
+        <v>29.070689999999999</v>
       </c>
       <c r="AH40" s="18">
         <f t="shared" si="3"/>
-        <v>94.024834408810534</v>
+        <v>-206.71600000000001</v>
       </c>
       <c r="AJ40" s="19" t="s">
         <v>79</v>
@@ -7467,7 +7465,7 @@
       </c>
       <c r="U41" s="8">
         <f t="shared" si="1"/>
-        <v>-17.968820611715174</v>
+        <v>0</v>
       </c>
       <c r="V41" s="8">
         <f t="shared" si="1"/>
@@ -7475,7 +7473,7 @@
       </c>
       <c r="W41" s="8">
         <f t="shared" si="1"/>
-        <v>4.0832277831392165</v>
+        <v>0</v>
       </c>
       <c r="X41" s="8">
         <f t="shared" si="1"/>
@@ -7491,7 +7489,7 @@
       </c>
       <c r="AA41" s="8">
         <f t="shared" si="1"/>
-        <v>240.07829999999998</v>
+        <v>0</v>
       </c>
       <c r="AB41" s="8">
         <f t="shared" si="1"/>
@@ -7515,11 +7513,11 @@
       </c>
       <c r="AG41" s="17">
         <f t="shared" si="1"/>
-        <v>62.974760000000003</v>
+        <v>31.487380000000002</v>
       </c>
       <c r="AH41" s="18">
         <f t="shared" si="3"/>
-        <v>106.67893717142402</v>
+        <v>-151.00115</v>
       </c>
       <c r="AJ41" s="19" t="s">
         <v>81</v>
@@ -7606,7 +7604,7 @@
       </c>
       <c r="U42" s="8">
         <f t="shared" si="1"/>
-        <v>-22.246496848178143</v>
+        <v>0</v>
       </c>
       <c r="V42" s="8">
         <f t="shared" si="1"/>
@@ -7614,7 +7612,7 @@
       </c>
       <c r="W42" s="8">
         <f t="shared" si="1"/>
-        <v>6.0353334055377585</v>
+        <v>0</v>
       </c>
       <c r="X42" s="8">
         <f t="shared" si="1"/>
@@ -7630,7 +7628,7 @@
       </c>
       <c r="AA42" s="8">
         <f t="shared" si="1"/>
-        <v>257.63330000000002</v>
+        <v>0</v>
       </c>
       <c r="AB42" s="8">
         <f t="shared" si="1"/>
@@ -7654,11 +7652,11 @@
       </c>
       <c r="AG42" s="17">
         <f t="shared" si="1"/>
-        <v>57.751620000000003</v>
+        <v>28.875810000000001</v>
       </c>
       <c r="AH42" s="18">
         <f t="shared" si="3"/>
-        <v>117.37091655735964</v>
+        <v>-152.92703</v>
       </c>
       <c r="AJ42" s="19" t="s">
         <v>83</v>
@@ -7745,7 +7743,7 @@
       </c>
       <c r="U43" s="8">
         <f t="shared" si="1"/>
-        <v>-23.1866419965462</v>
+        <v>0</v>
       </c>
       <c r="V43" s="8">
         <f t="shared" si="1"/>
@@ -7753,7 +7751,7 @@
       </c>
       <c r="W43" s="8">
         <f t="shared" si="1"/>
-        <v>14.519882481652528</v>
+        <v>0</v>
       </c>
       <c r="X43" s="8">
         <f t="shared" si="1"/>
@@ -7769,7 +7767,7 @@
       </c>
       <c r="AA43" s="8">
         <f t="shared" si="1"/>
-        <v>268.47090000000003</v>
+        <v>0</v>
       </c>
       <c r="AB43" s="8">
         <f t="shared" si="1"/>
@@ -7793,11 +7791,11 @@
       </c>
       <c r="AG43" s="17">
         <f t="shared" si="1"/>
-        <v>58.00694</v>
+        <v>29.00347</v>
       </c>
       <c r="AH43" s="18">
         <f t="shared" si="3"/>
-        <v>104.93585048510637</v>
+        <v>-183.87175999999999</v>
       </c>
       <c r="AJ43" s="19" t="s">
         <v>85</v>
@@ -7884,7 +7882,7 @@
       </c>
       <c r="U44" s="8">
         <f t="shared" si="4"/>
-        <v>-19.819733348988326</v>
+        <v>0</v>
       </c>
       <c r="V44" s="8">
         <f t="shared" si="4"/>
@@ -7892,7 +7890,7 @@
       </c>
       <c r="W44" s="8">
         <f t="shared" si="4"/>
-        <v>6.3393864025629485</v>
+        <v>0</v>
       </c>
       <c r="X44" s="8">
         <f t="shared" si="4"/>
@@ -7908,7 +7906,7 @@
       </c>
       <c r="AA44" s="8">
         <f t="shared" si="4"/>
-        <v>252.3862</v>
+        <v>0</v>
       </c>
       <c r="AB44" s="8">
         <f t="shared" si="4"/>
@@ -7932,11 +7930,11 @@
       </c>
       <c r="AG44" s="17">
         <f t="shared" si="4"/>
-        <v>53.812440000000002</v>
+        <v>26.906220000000001</v>
       </c>
       <c r="AH44" s="18">
         <f t="shared" si="3"/>
-        <v>99.71427305357463</v>
+        <v>-166.09780000000001</v>
       </c>
       <c r="AJ44" s="19" t="s">
         <v>87</v>
@@ -8023,7 +8021,7 @@
       </c>
       <c r="U45" s="8">
         <f t="shared" si="4"/>
-        <v>-18.419571669395573</v>
+        <v>0</v>
       </c>
       <c r="V45" s="8">
         <f t="shared" si="4"/>
@@ -8031,7 +8029,7 @@
       </c>
       <c r="W45" s="8">
         <f t="shared" si="4"/>
-        <v>19.497339141534162</v>
+        <v>0</v>
       </c>
       <c r="X45" s="8">
         <f t="shared" si="4"/>
@@ -8047,7 +8045,7 @@
       </c>
       <c r="AA45" s="8">
         <f t="shared" si="4"/>
-        <v>238.61189999999999</v>
+        <v>0</v>
       </c>
       <c r="AB45" s="8">
         <f t="shared" si="4"/>
@@ -8071,11 +8069,11 @@
       </c>
       <c r="AG45" s="17">
         <f t="shared" si="4"/>
-        <v>58.239919999999998</v>
+        <v>29.119959999999999</v>
       </c>
       <c r="AH45" s="18">
         <f t="shared" si="3"/>
-        <v>109.31179747213857</v>
+        <v>-159.49783000000002</v>
       </c>
       <c r="AJ45" s="19" t="s">
         <v>89</v>
@@ -8162,7 +8160,7 @@
       </c>
       <c r="U46" s="8">
         <f t="shared" si="4"/>
-        <v>-22.009073041452702</v>
+        <v>0</v>
       </c>
       <c r="V46" s="8">
         <f t="shared" si="4"/>
@@ -8170,7 +8168,7 @@
       </c>
       <c r="W46" s="8">
         <f t="shared" si="4"/>
-        <v>8.5495338820312305</v>
+        <v>0</v>
       </c>
       <c r="X46" s="8">
         <f t="shared" si="4"/>
@@ -8186,7 +8184,7 @@
       </c>
       <c r="AA46" s="8">
         <f t="shared" si="4"/>
-        <v>250.15109999999999</v>
+        <v>0</v>
       </c>
       <c r="AB46" s="8">
         <f t="shared" si="4"/>
@@ -8210,11 +8208,11 @@
       </c>
       <c r="AG46" s="17">
         <f t="shared" si="4"/>
-        <v>57.682099999999998</v>
+        <v>28.841049999999999</v>
       </c>
       <c r="AH46" s="18">
         <f t="shared" si="3"/>
-        <v>110.7739808405785</v>
+        <v>-154.75863000000001</v>
       </c>
       <c r="AJ46" s="19" t="s">
         <v>91</v>
@@ -8301,7 +8299,7 @@
       </c>
       <c r="U47" s="8">
         <f t="shared" si="4"/>
-        <v>-8.2025371543809538</v>
+        <v>0</v>
       </c>
       <c r="V47" s="8">
         <f t="shared" si="4"/>
@@ -8309,7 +8307,7 @@
       </c>
       <c r="W47" s="8">
         <f t="shared" si="4"/>
-        <v>3.4483689200838126</v>
+        <v>0</v>
       </c>
       <c r="X47" s="8">
         <f t="shared" si="4"/>
@@ -8325,7 +8323,7 @@
       </c>
       <c r="AA47" s="8">
         <f t="shared" si="4"/>
-        <v>257.91570000000002</v>
+        <v>0</v>
       </c>
       <c r="AB47" s="8">
         <f t="shared" si="4"/>
@@ -8349,11 +8347,11 @@
       </c>
       <c r="AG47" s="17">
         <f t="shared" si="4"/>
-        <v>58.795319999999997</v>
+        <v>29.397659999999998</v>
       </c>
       <c r="AH47" s="18">
         <f t="shared" si="3"/>
-        <v>80.870431765702875</v>
+        <v>-201.68876</v>
       </c>
       <c r="AJ47" s="19" t="s">
         <v>93</v>
@@ -8440,7 +8438,7 @@
       </c>
       <c r="U48" s="8">
         <f t="shared" si="4"/>
-        <v>-8.3092640254116361</v>
+        <v>0</v>
       </c>
       <c r="V48" s="8">
         <f t="shared" si="4"/>
@@ -8448,7 +8446,7 @@
       </c>
       <c r="W48" s="8">
         <f t="shared" si="4"/>
-        <v>7.3429984635705878</v>
+        <v>0</v>
       </c>
       <c r="X48" s="8">
         <f t="shared" si="4"/>
@@ -8464,7 +8462,7 @@
       </c>
       <c r="AA48" s="8">
         <f t="shared" si="4"/>
-        <v>255.9873</v>
+        <v>0</v>
       </c>
       <c r="AB48" s="8">
         <f t="shared" si="4"/>
@@ -8488,11 +8486,11 @@
       </c>
       <c r="AG48" s="17">
         <f t="shared" si="4"/>
-        <v>52.749360000000003</v>
+        <v>26.374680000000001</v>
       </c>
       <c r="AH48" s="18">
         <f t="shared" si="3"/>
-        <v>68.983404438158942</v>
+        <v>-212.41230999999999</v>
       </c>
       <c r="AJ48" s="19" t="s">
         <v>95</v>
@@ -8579,7 +8577,7 @@
       </c>
       <c r="U49" s="8">
         <f t="shared" si="4"/>
-        <v>-4.5404615100229631</v>
+        <v>0</v>
       </c>
       <c r="V49" s="8">
         <f t="shared" si="4"/>
@@ -8587,7 +8585,7 @@
       </c>
       <c r="W49" s="8">
         <f t="shared" si="4"/>
-        <v>4.3865218335259657</v>
+        <v>0</v>
       </c>
       <c r="X49" s="8">
         <f t="shared" si="4"/>
@@ -8603,7 +8601,7 @@
       </c>
       <c r="AA49" s="8">
         <f t="shared" si="4"/>
-        <v>225.48320000000001</v>
+        <v>0</v>
       </c>
       <c r="AB49" s="8">
         <f t="shared" si="4"/>
@@ -8627,11 +8625,11 @@
       </c>
       <c r="AG49" s="17">
         <f t="shared" si="4"/>
-        <v>57.932920000000003</v>
+        <v>28.966460000000001</v>
       </c>
       <c r="AH49" s="18">
         <f t="shared" si="3"/>
-        <v>78.117700323503016</v>
+        <v>-176.17801999999998</v>
       </c>
       <c r="AJ49" s="19" t="s">
         <v>97</v>
@@ -8718,7 +8716,7 @@
       </c>
       <c r="U50" s="8">
         <f t="shared" si="4"/>
-        <v>-6.3763850511869187</v>
+        <v>0</v>
       </c>
       <c r="V50" s="8">
         <f t="shared" si="4"/>
@@ -8726,7 +8724,7 @@
       </c>
       <c r="W50" s="8">
         <f t="shared" si="4"/>
-        <v>7.489475164789587</v>
+        <v>0</v>
       </c>
       <c r="X50" s="8">
         <f t="shared" si="4"/>
@@ -8742,7 +8740,7 @@
       </c>
       <c r="AA50" s="8">
         <f t="shared" si="4"/>
-        <v>205.99509999999998</v>
+        <v>0</v>
       </c>
       <c r="AB50" s="8">
         <f t="shared" si="4"/>
@@ -8766,11 +8764,11 @@
       </c>
       <c r="AG50" s="17">
         <f t="shared" si="4"/>
-        <v>52.632339999999999</v>
+        <v>26.31617</v>
       </c>
       <c r="AH50" s="18">
         <f t="shared" si="3"/>
-        <v>52.782160113602629</v>
+        <v>-180.6422</v>
       </c>
       <c r="AJ50" s="19" t="s">
         <v>99</v>
@@ -8857,7 +8855,7 @@
       </c>
       <c r="U51" s="8">
         <f t="shared" si="4"/>
-        <v>-13.937043086106897</v>
+        <v>0</v>
       </c>
       <c r="V51" s="8">
         <f t="shared" si="4"/>
@@ -8865,7 +8863,7 @@
       </c>
       <c r="W51" s="8">
         <f t="shared" si="4"/>
-        <v>1.5142882803482303</v>
+        <v>0</v>
       </c>
       <c r="X51" s="8">
         <f t="shared" si="4"/>
@@ -8881,7 +8879,7 @@
       </c>
       <c r="AA51" s="8">
         <f t="shared" si="4"/>
-        <v>269.03980000000001</v>
+        <v>0</v>
       </c>
       <c r="AB51" s="8">
         <f t="shared" si="4"/>
@@ -8905,11 +8903,11 @@
       </c>
       <c r="AG51" s="17">
         <f t="shared" si="4"/>
-        <v>54.944099999999999</v>
+        <v>27.472049999999999</v>
       </c>
       <c r="AH51" s="18">
         <f t="shared" si="3"/>
-        <v>97.747265194241322</v>
+        <v>-186.34183000000002</v>
       </c>
       <c r="AJ51" s="19" t="s">
         <v>101</v>
@@ -8996,7 +8994,7 @@
       </c>
       <c r="U52" s="8">
         <f t="shared" si="4"/>
-        <v>2.9977443535098187</v>
+        <v>0</v>
       </c>
       <c r="V52" s="8">
         <f t="shared" si="4"/>
@@ -9004,7 +9002,7 @@
       </c>
       <c r="W52" s="8">
         <f t="shared" si="4"/>
-        <v>-1.6877075872318641</v>
+        <v>0</v>
       </c>
       <c r="X52" s="8">
         <f t="shared" si="4"/>
@@ -9020,7 +9018,7 @@
       </c>
       <c r="AA52" s="8">
         <f t="shared" si="4"/>
-        <v>256.08670000000001</v>
+        <v>0</v>
       </c>
       <c r="AB52" s="8">
         <f t="shared" si="4"/>
@@ -9044,11 +9042,11 @@
       </c>
       <c r="AG52" s="17">
         <f t="shared" si="4"/>
-        <v>57.849559999999997</v>
+        <v>28.924779999999998</v>
       </c>
       <c r="AH52" s="18">
         <f t="shared" si="3"/>
-        <v>101.21340676627796</v>
+        <v>-185.10811000000001</v>
       </c>
       <c r="AJ52" s="19" t="s">
         <v>103</v>
@@ -9135,7 +9133,7 @@
       </c>
       <c r="U53" s="8">
         <f t="shared" si="6"/>
-        <v>-18.420583598246829</v>
+        <v>0</v>
       </c>
       <c r="V53" s="8">
         <f t="shared" si="6"/>
@@ -9143,7 +9141,7 @@
       </c>
       <c r="W53" s="8">
         <f t="shared" si="6"/>
-        <v>2.5766238375051955</v>
+        <v>0</v>
       </c>
       <c r="X53" s="8">
         <f t="shared" si="6"/>
@@ -9159,7 +9157,7 @@
       </c>
       <c r="AA53" s="8">
         <f t="shared" si="6"/>
-        <v>257.16339999999997</v>
+        <v>0</v>
       </c>
       <c r="AB53" s="8">
         <f t="shared" si="6"/>
@@ -9183,11 +9181,11 @@
       </c>
       <c r="AG53" s="17">
         <f t="shared" si="6"/>
-        <v>65.169399999999996</v>
+        <v>32.584699999999998</v>
       </c>
       <c r="AH53" s="18">
         <f t="shared" si="3"/>
-        <v>97.079300239258345</v>
+        <v>-176.82483999999999</v>
       </c>
       <c r="AJ53" s="19" t="s">
         <v>105</v>
@@ -9274,7 +9272,7 @@
       </c>
       <c r="U54" s="8">
         <f t="shared" si="6"/>
-        <v>9.1992238273128244</v>
+        <v>0</v>
       </c>
       <c r="V54" s="8">
         <f t="shared" si="6"/>
@@ -9282,7 +9280,7 @@
       </c>
       <c r="W54" s="8">
         <f t="shared" si="6"/>
-        <v>4.1491612723537274</v>
+        <v>0</v>
       </c>
       <c r="X54" s="8">
         <f t="shared" si="6"/>
@@ -9298,7 +9296,7 @@
       </c>
       <c r="AA54" s="8">
         <f t="shared" si="6"/>
-        <v>227.79589999999999</v>
+        <v>0</v>
       </c>
       <c r="AB54" s="8">
         <f t="shared" si="6"/>
@@ -9322,11 +9320,11 @@
       </c>
       <c r="AG54" s="17">
         <f t="shared" si="6"/>
-        <v>55.261679999999998</v>
+        <v>27.630839999999999</v>
       </c>
       <c r="AH54" s="18">
         <f t="shared" si="3"/>
-        <v>105.73284509966653</v>
+        <v>-163.04228000000001</v>
       </c>
       <c r="AJ54" s="19" t="s">
         <v>107</v>
@@ -9413,7 +9411,7 @@
       </c>
       <c r="U55" s="8">
         <f t="shared" si="6"/>
-        <v>-38.819013759045973</v>
+        <v>0</v>
       </c>
       <c r="V55" s="8">
         <f t="shared" si="6"/>
@@ -9421,7 +9419,7 @@
       </c>
       <c r="W55" s="8">
         <f t="shared" si="6"/>
-        <v>237.3055375409516</v>
+        <v>0</v>
       </c>
       <c r="X55" s="8">
         <f t="shared" si="6"/>
@@ -9437,7 +9435,7 @@
       </c>
       <c r="AA55" s="8">
         <f t="shared" si="6"/>
-        <v>314.76679999999999</v>
+        <v>0</v>
       </c>
       <c r="AB55" s="8">
         <f t="shared" si="6"/>
@@ -9461,11 +9459,11 @@
       </c>
       <c r="AG55" s="17">
         <f t="shared" si="6"/>
-        <v>64.569239999999994</v>
+        <v>32.284619999999997</v>
       </c>
       <c r="AH55" s="18">
         <f t="shared" si="3"/>
-        <v>277.32570378190559</v>
+        <v>-268.21224000000001</v>
       </c>
       <c r="AJ55" s="19" t="s">
         <v>109</v>
@@ -9552,7 +9550,7 @@
       </c>
       <c r="U56" s="8">
         <f t="shared" si="6"/>
-        <v>-28.363037544029027</v>
+        <v>0</v>
       </c>
       <c r="V56" s="8">
         <f t="shared" si="6"/>
@@ -9560,7 +9558,7 @@
       </c>
       <c r="W56" s="8">
         <f t="shared" si="6"/>
-        <v>264.56386500717741</v>
+        <v>0</v>
       </c>
       <c r="X56" s="8">
         <f t="shared" si="6"/>
@@ -9576,7 +9574,7 @@
       </c>
       <c r="AA56" s="8">
         <f t="shared" si="6"/>
-        <v>267.80219999999997</v>
+        <v>0</v>
       </c>
       <c r="AB56" s="8">
         <f t="shared" si="6"/>
@@ -9600,11 +9598,11 @@
       </c>
       <c r="AG56" s="17">
         <f t="shared" si="6"/>
-        <v>67.451480000000004</v>
+        <v>33.725740000000002</v>
       </c>
       <c r="AH56" s="18">
         <f t="shared" si="3"/>
-        <v>310.29476746314833</v>
+        <v>-227.434</v>
       </c>
       <c r="AJ56" s="19" t="s">
         <v>111</v>
@@ -9691,7 +9689,7 @@
       </c>
       <c r="U57" s="8">
         <f t="shared" si="6"/>
-        <v>-26.97862400718391</v>
+        <v>0</v>
       </c>
       <c r="V57" s="8">
         <f t="shared" si="6"/>
@@ -9699,7 +9697,7 @@
       </c>
       <c r="W57" s="8">
         <f t="shared" si="6"/>
-        <v>8.9969329253918531</v>
+        <v>0</v>
       </c>
       <c r="X57" s="8">
         <f t="shared" si="6"/>
@@ -9715,7 +9713,7 @@
       </c>
       <c r="AA57" s="8">
         <f t="shared" si="6"/>
-        <v>282.38260000000002</v>
+        <v>0</v>
       </c>
       <c r="AB57" s="8">
         <f t="shared" si="6"/>
@@ -9739,11 +9737,11 @@
       </c>
       <c r="AG57" s="17">
         <f t="shared" si="6"/>
-        <v>63.074480000000001</v>
+        <v>31.537240000000001</v>
       </c>
       <c r="AH57" s="18">
         <f t="shared" si="3"/>
-        <v>118.33703891820798</v>
+        <v>-177.60111000000001</v>
       </c>
       <c r="AJ57" s="19" t="s">
         <v>113</v>
@@ -9830,7 +9828,7 @@
       </c>
       <c r="U58" s="8">
         <f t="shared" si="6"/>
-        <v>-23.185883049907762</v>
+        <v>0</v>
       </c>
       <c r="V58" s="8">
         <f t="shared" si="6"/>
@@ -9838,7 +9836,7 @@
       </c>
       <c r="W58" s="8">
         <f t="shared" si="6"/>
-        <v>4.8485305996765655</v>
+        <v>0</v>
       </c>
       <c r="X58" s="8">
         <f t="shared" si="6"/>
@@ -9854,7 +9852,7 @@
       </c>
       <c r="AA58" s="8">
         <f t="shared" si="6"/>
-        <v>290.30279999999999</v>
+        <v>0</v>
       </c>
       <c r="AB58" s="8">
         <f t="shared" si="6"/>
@@ -9878,11 +9876,11 @@
       </c>
       <c r="AG58" s="17">
         <f t="shared" si="6"/>
-        <v>49.265920000000001</v>
+        <v>24.632960000000001</v>
       </c>
       <c r="AH58" s="18">
         <f t="shared" si="3"/>
-        <v>103.44681754976878</v>
+        <v>-193.15159</v>
       </c>
       <c r="AJ58" s="19" t="s">
         <v>115</v>
@@ -9969,7 +9967,7 @@
       </c>
       <c r="U59" s="21">
         <f t="shared" si="6"/>
-        <v>-13.755812953402646</v>
+        <v>0</v>
       </c>
       <c r="V59" s="21">
         <f t="shared" si="6"/>
@@ -9977,7 +9975,7 @@
       </c>
       <c r="W59" s="21">
         <f t="shared" si="6"/>
-        <v>-4.1275312931581754</v>
+        <v>0</v>
       </c>
       <c r="X59" s="21">
         <f t="shared" si="6"/>
@@ -9993,7 +9991,7 @@
       </c>
       <c r="AA59" s="21">
         <f t="shared" si="6"/>
-        <v>266.01800000000003</v>
+        <v>0</v>
       </c>
       <c r="AB59" s="21">
         <f t="shared" si="6"/>
@@ -10017,11 +10015,11 @@
       </c>
       <c r="AG59" s="22">
         <f t="shared" si="6"/>
-        <v>50.306919999999998</v>
+        <v>25.153459999999999</v>
       </c>
       <c r="AH59" s="18">
         <f t="shared" si="3"/>
-        <v>60.570235753439199</v>
+        <v>-212.71788000000001</v>
       </c>
       <c r="AJ59" s="19" t="s">
         <v>117</v>
@@ -10255,17 +10253,17 @@
       <c r="D62" s="55"/>
       <c r="E62" s="61">
         <f>MAX(AH35:AH59)</f>
-        <v>310.29476746314833</v>
+        <v>-151.00115</v>
       </c>
       <c r="F62" s="62"/>
       <c r="G62" s="34">
         <f>_xlfn.XLOOKUP(MAX(AH35:AH59),AH35:AH59,B35:B59)</f>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H62" s="35"/>
       <c r="I62" s="34" t="str">
         <f>_xlfn.XLOOKUP(MAX(AH35:AH59),AH35:AH59,AK35:AK59)</f>
-        <v>CeSbL</v>
+        <v>PoBw</v>
       </c>
       <c r="J62" s="35"/>
       <c r="BJ62" s="24">
@@ -12713,325 +12711,11 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="N5 W5" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005EDA4EBA40014468BD70616C7A96D14" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="50721e4afd631f278bee133812e5fef0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="051e4247-5afa-41d6-9ecb-95bb5262d825" xmlns:ns3="1bccae83-48d9-4882-b875-c21b283dc0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="879b5544f3aba6c4b909f13333d8de76" ns2:_="" ns3:_="">
-    <xsd:import namespace="051e4247-5afa-41d6-9ecb-95bb5262d825"/>
-    <xsd:import namespace="1bccae83-48d9-4882-b875-c21b283dc0ec"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:ToPerson" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:Comments" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="051e4247-5afa-41d6-9ecb-95bb5262d825" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ToPerson" ma:index="10" nillable="true" ma:displayName="To Person" ma:description="The file was intended for this individual" ma:format="Dropdown" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="ToPerson">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="12" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Comments" ma:index="13" nillable="true" ma:displayName="Comments" ma:description="comments, description, purpose, etc" ma:format="Dropdown" ma:internalName="Comments">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="16" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c03f8475-640f-4944-9dcc-2d3788384b7c" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="21" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="22" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="23" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="25" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="26" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1bccae83-48d9-4882-b875-c21b283dc0ec" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f515cb03-89b1-45a4-9671-02e9b54e5b85}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="1bccae83-48d9-4882-b875-c21b283dc0ec">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="051e4247-5afa-41d6-9ecb-95bb5262d825" xsi:nil="true"/>
-    <TaxCatchAll xmlns="1bccae83-48d9-4882-b875-c21b283dc0ec" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="051e4247-5afa-41d6-9ecb-95bb5262d825">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <ToPerson xmlns="051e4247-5afa-41d6-9ecb-95bb5262d825">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </ToPerson>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE72F18-86F8-48BA-A940-13F2294F8271}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31881EA9-49CB-48AE-9101-8BED38825D25}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E39570D2-4AFB-48ED-BB95-E5C2EA11C35C}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
added fec ecosite reference doc
</commit_message>
<xml_diff>
--- a/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
+++ b/Misc/FEC_EcositePredictor/reference/FEC_EcositePredictor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MNR_SR_External\GI_MGMT\GISupport\OldGrowthAnalysis\Documents_GWatt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/glen_watt_ontario_ca/Documents/Laptop_Feb2024/SR_RIAU_toolbox/p2t_ArcMap10_Tools-master/p2t_ArcMap10_Tools-master/Misc/FEC_EcositePredictor/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D49DB22-8E40-4DB3-B13C-5C8D86E14300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{5D49DB22-8E40-4DB3-B13C-5C8D86E14300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B8DAAA8-9437-4E37-A7B5-B7378D660AB1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{81CC09A0-CCBA-490A-882D-74783881A46D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="166">
   <si>
     <t>Ecosite_Num</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>SITE CLASS</t>
+  </si>
+  <si>
+    <t>OC</t>
   </si>
 </sst>
 </file>
@@ -3136,19 +3139,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BAB770-D548-4A89-9CE4-B3603514F2DA}">
-  <dimension ref="B1:Z9"/>
+  <dimension ref="B1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="25" max="25" width="3.42578125" customWidth="1"/>
-    <col min="26" max="26" width="12" customWidth="1"/>
+    <col min="26" max="26" width="3.42578125" customWidth="1"/>
+    <col min="27" max="27" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="47" t="s">
         <v>163</v>
       </c>
@@ -3173,12 +3176,13 @@
       <c r="U2" s="48"/>
       <c r="V2" s="48"/>
       <c r="W2" s="48"/>
-      <c r="X2" s="49"/>
-      <c r="Z2" s="39" t="s">
+      <c r="X2" s="48"/>
+      <c r="Y2" s="49"/>
+      <c r="AA2" s="39" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
         <v>44</v>
       </c>
@@ -3207,50 +3211,53 @@
         <v>156</v>
       </c>
       <c r="K3" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="M3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="N3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="O3" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="P3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="Q3" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="R3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="S3" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="T3" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="U3" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="V3" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="W3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="32" t="s">
+      <c r="X3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="28" t="s">
+      <c r="Y3" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
     </row>
-    <row r="4" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29">
         <v>0</v>
       </c>
@@ -3314,17 +3321,20 @@
       <c r="V4" s="30">
         <v>0</v>
       </c>
-      <c r="W4" s="33">
-        <v>0</v>
-      </c>
-      <c r="X4" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="38">
-        <v>1</v>
+      <c r="W4" s="30">
+        <v>0</v>
+      </c>
+      <c r="X4" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="31">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="38">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0</v>
       </c>
@@ -3394,38 +3404,41 @@
       <c r="X5">
         <v>0</v>
       </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:26" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="K8" s="41" t="s">
+    <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:27" ht="22.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L8" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="43" t="s">
+      <c r="M8" s="42"/>
+      <c r="N8" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
     </row>
-    <row r="9" spans="2:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K9" s="44">
+    <row r="9" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="44">
         <f>'Central Ontario FEC'!G62</f>
         <v>17</v>
       </c>
-      <c r="L9" s="45"/>
-      <c r="M9" s="46" t="str">
+      <c r="M9" s="45"/>
+      <c r="N9" s="46" t="str">
         <f>'Central Ontario FEC'!I62</f>
         <v>PoBw</v>
       </c>
-      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="B2:X2"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="B2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3656,47 +3669,47 @@
         <v>1</v>
       </c>
       <c r="D4" s="6">
+        <f>'User Entry'!N4</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <f>'User Entry'!Q4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <f>'User Entry'!P4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <f>'User Entry'!W4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <f>'User Entry'!O4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <f>'User Entry'!R4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <f>'User Entry'!T4+'User Entry'!V4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <f>'User Entry'!X4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <f>'User Entry'!L4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
         <f>'User Entry'!M4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="6">
-        <f>'User Entry'!P4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <f>'User Entry'!O4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <f>'User Entry'!V4</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <f>'User Entry'!N4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <f>'User Entry'!Q4</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="N4" s="6">
         <f>'User Entry'!S4+'User Entry'!U4</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <f>'User Entry'!W4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <f>'User Entry'!K4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <f>'User Entry'!L4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <f>'User Entry'!R4+'User Entry'!T4</f>
         <v>0</v>
       </c>
       <c r="O4" s="6">
@@ -3740,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="6">
-        <f>G4+H4+I4+J4+K4+N4+'User Entry'!X4</f>
+        <f>G4+H4+I4+J4+K4+N4+'User Entry'!Y4</f>
         <v>0</v>
       </c>
       <c r="Z4" s="6">
@@ -3748,7 +3761,7 @@
         <v>0</v>
       </c>
       <c r="AA4" s="6">
-        <f>O4+P4+Q4+R4+S4+T4+U4+V4+W4</f>
+        <f>O4+P4+Q4+R4+S4+T4+U4+V4+W4+'User Entry'!K4</f>
         <v>0</v>
       </c>
       <c r="AB4" s="6"/>
@@ -3757,8 +3770,8 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6">
-        <f>'User Entry'!Z4</f>
-        <v>1</v>
+        <f>'User Entry'!AA4</f>
+        <v>0</v>
       </c>
       <c r="AP4" s="25">
         <f>SUM(D4:M4,O4:V4)</f>

</xml_diff>